<commit_message>
Update task time, active time, and finger movement statistics
</commit_message>
<xml_diff>
--- a/Evaluation/src/Replico Evaluation Results.xlsx
+++ b/Evaluation/src/Replico Evaluation Results.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunom\Documents\Unity\orpheus\Evaluation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D03E9AD-3988-4A66-8313-CF92DCB9255A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AC4EAB-FC3A-4124-A7CB-FA29FF919EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{FD735BD4-5F7E-446F-A7DD-88F8AEB01BC1}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profiling" sheetId="1" r:id="rId1"/>
@@ -586,7 +585,6 @@
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1533,9 +1531,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="1">
-      <selection activeCell="U21" sqref="U21:AA21"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3424,9 +3419,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2:N2"/>
     </sheetView>
-    <sheetView topLeftCell="M1" workbookViewId="1">
-      <selection activeCell="U21" sqref="U21:Z21"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5312,7 +5304,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5:D81"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7691,10 +7682,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F69" sqref="F69"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10068,15 +10058,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AG209"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11:Y101"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10184,7 +10173,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -10292,7 +10281,7 @@
         <v>53.318069999999992</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -10400,7 +10389,7 @@
         <v>30.24963</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -10508,7 +10497,7 @@
         <v>92.076480000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -10616,7 +10605,7 @@
         <v>42.917480000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -10724,7 +10713,7 @@
         <v>41.570989999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -10832,7 +10821,7 @@
         <v>83.967039999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -10940,7 +10929,7 @@
         <v>31.772709999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -11048,7 +11037,7 @@
         <v>215.22139000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -11264,7 +11253,7 @@
         <v>48.827145000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -11372,7 +11361,7 @@
         <v>31.015619999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -11480,7 +11469,7 @@
         <v>20.779539000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -11588,7 +11577,7 @@
         <v>82.426270000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -11696,7 +11685,7 @@
         <v>16.305172999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -11804,7 +11793,7 @@
         <v>32.03931</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -11912,7 +11901,7 @@
         <v>39.397950000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -12020,7 +12009,7 @@
         <v>26.834959999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>2</v>
       </c>
@@ -12128,7 +12117,7 @@
         <v>64.579589999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>2</v>
       </c>
@@ -12344,7 +12333,7 @@
         <v>36.374749999999992</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>3</v>
       </c>
@@ -12452,7 +12441,7 @@
         <v>56.85718</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>3</v>
       </c>
@@ -12560,7 +12549,7 @@
         <v>23.057864000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>3</v>
       </c>
@@ -12668,7 +12657,7 @@
         <v>107.89623999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>3</v>
       </c>
@@ -12776,7 +12765,7 @@
         <v>17.480713000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>3</v>
       </c>
@@ -12884,7 +12873,7 @@
         <v>74.494139999999987</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>3</v>
       </c>
@@ -12992,7 +12981,7 @@
         <v>34.768070000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>3</v>
       </c>
@@ -13100,7 +13089,7 @@
         <v>36.881100000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>3</v>
       </c>
@@ -13208,7 +13197,7 @@
         <v>54.036869999999993</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>3</v>
       </c>
@@ -13424,7 +13413,7 @@
         <v>88.918700000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>4</v>
       </c>
@@ -13532,7 +13521,7 @@
         <v>76.159669999999991</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>4</v>
       </c>
@@ -13640,7 +13629,7 @@
         <v>82.986809999999991</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>4</v>
       </c>
@@ -13748,7 +13737,7 @@
         <v>92.330560000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>4</v>
       </c>
@@ -13856,7 +13845,7 @@
         <v>38.27637</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>4</v>
       </c>
@@ -13964,7 +13953,7 @@
         <v>24.597169999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>4</v>
       </c>
@@ -14072,7 +14061,7 @@
         <v>27.61523</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>4</v>
       </c>
@@ -14180,7 +14169,7 @@
         <v>32.729979999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>4</v>
       </c>
@@ -14288,7 +14277,7 @@
         <v>81.385250000000013</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>4</v>
       </c>
@@ -14504,7 +14493,7 @@
         <v>40.211910000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>5</v>
       </c>
@@ -14612,7 +14601,7 @@
         <v>76.444329999999994</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>5</v>
       </c>
@@ -14720,7 +14709,7 @@
         <v>97.914059999999992</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>5</v>
       </c>
@@ -14828,7 +14817,7 @@
         <v>153.85005999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>5</v>
       </c>
@@ -14936,7 +14925,7 @@
         <v>31.575679999999991</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>5</v>
       </c>
@@ -15044,7 +15033,7 @@
         <v>129.95068999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>5</v>
       </c>
@@ -15152,7 +15141,7 @@
         <v>39.419429999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>5</v>
       </c>
@@ -15260,7 +15249,7 @@
         <v>35.250979999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>5</v>
       </c>
@@ -15368,7 +15357,7 @@
         <v>258.70751999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>5</v>
       </c>
@@ -15584,7 +15573,7 @@
         <v>82.201660000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>6</v>
       </c>
@@ -15692,7 +15681,7 @@
         <v>46.864019999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>6</v>
       </c>
@@ -15800,7 +15789,7 @@
         <v>23.15991</v>
       </c>
     </row>
-    <row r="54" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>6</v>
       </c>
@@ -15908,7 +15897,7 @@
         <v>92.6875</v>
       </c>
     </row>
-    <row r="55" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>6</v>
       </c>
@@ -16016,7 +16005,7 @@
         <v>17.377441999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>6</v>
       </c>
@@ -16124,7 +16113,7 @@
         <v>18.179194000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>6</v>
       </c>
@@ -16232,7 +16221,7 @@
         <v>41.199220000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>6</v>
       </c>
@@ -16340,7 +16329,7 @@
         <v>26.496091999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>6</v>
       </c>
@@ -16448,7 +16437,7 @@
         <v>173.39937999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>6</v>
       </c>
@@ -16664,7 +16653,7 @@
         <v>22.653315999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>7</v>
       </c>
@@ -16772,7 +16761,7 @@
         <v>103.48731000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>7</v>
       </c>
@@ -16880,7 +16869,7 @@
         <v>69.674800000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>7</v>
       </c>
@@ -16988,7 +16977,7 @@
         <v>163.71875</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>7</v>
       </c>
@@ -17096,7 +17085,7 @@
         <v>30.060546000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>7</v>
       </c>
@@ -17204,7 +17193,7 @@
         <v>167.47069999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>7</v>
       </c>
@@ -17312,7 +17301,7 @@
         <v>237.01754</v>
       </c>
     </row>
-    <row r="68" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>7</v>
       </c>
@@ -17420,7 +17409,7 @@
         <v>158.03710999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>7</v>
       </c>
@@ -17528,7 +17517,7 @@
         <v>295.35149999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>7</v>
       </c>
@@ -17744,7 +17733,7 @@
         <v>323.73040000000003</v>
       </c>
     </row>
-    <row r="72" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>8</v>
       </c>
@@ -17852,7 +17841,7 @@
         <v>33.814450000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>8</v>
       </c>
@@ -17960,7 +17949,7 @@
         <v>23.333987</v>
       </c>
     </row>
-    <row r="74" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>8</v>
       </c>
@@ -18068,7 +18057,7 @@
         <v>72.375</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>8</v>
       </c>
@@ -18176,7 +18165,7 @@
         <v>40.949710000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>8</v>
       </c>
@@ -18284,7 +18273,7 @@
         <v>86.09863</v>
       </c>
     </row>
-    <row r="77" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>8</v>
       </c>
@@ -18392,7 +18381,7 @@
         <v>29.6416</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>8</v>
       </c>
@@ -18500,7 +18489,7 @@
         <v>25.485348000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>8</v>
       </c>
@@ -18608,7 +18597,7 @@
         <v>76.155270000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>8</v>
       </c>
@@ -18824,7 +18813,7 @@
         <v>130.93116000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>9</v>
       </c>
@@ -18932,7 +18921,7 @@
         <v>56.186520999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>9</v>
       </c>
@@ -19040,7 +19029,7 @@
         <v>31.188969999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>9</v>
       </c>
@@ -19148,7 +19137,7 @@
         <v>182.48687000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>9</v>
       </c>
@@ -19256,7 +19245,7 @@
         <v>84.381349999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>9</v>
       </c>
@@ -19364,7 +19353,7 @@
         <v>212.73586</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>9</v>
       </c>
@@ -19472,7 +19461,7 @@
         <v>290.0224</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>9</v>
       </c>
@@ -19580,7 +19569,7 @@
         <v>155.86324999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>9</v>
       </c>
@@ -19688,7 +19677,7 @@
         <v>286.01902999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>9</v>
       </c>
@@ -19904,7 +19893,7 @@
         <v>387.13130000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>10</v>
       </c>
@@ -20012,7 +20001,7 @@
         <v>72.458979999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>10</v>
       </c>
@@ -20120,7 +20109,7 @@
         <v>31.316405</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>10</v>
       </c>
@@ -20228,7 +20217,7 @@
         <v>74.671869999999984</v>
       </c>
     </row>
-    <row r="95" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>10</v>
       </c>
@@ -20336,7 +20325,7 @@
         <v>25.332032999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>10</v>
       </c>
@@ -20444,7 +20433,7 @@
         <v>25.136719399999997</v>
       </c>
     </row>
-    <row r="97" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>10</v>
       </c>
@@ -20552,7 +20541,7 @@
         <v>33.236327000000003</v>
       </c>
     </row>
-    <row r="98" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>10</v>
       </c>
@@ -20660,7 +20649,7 @@
         <v>51.476570000000002</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>10</v>
       </c>
@@ -20768,7 +20757,7 @@
         <v>103.30077999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>10</v>
       </c>
@@ -21523,7 +21512,13 @@
       <c r="A209" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE101" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <autoFilter ref="A1:AE101" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="7"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -21531,15 +21526,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AG101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2:AG101"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21647,7 +21641,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -21755,7 +21749,7 @@
         <v>27.645510000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -21863,7 +21857,7 @@
         <v>31.140989999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -21971,7 +21965,7 @@
         <v>50.346559999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -22079,7 +22073,7 @@
         <v>22.130862</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -22187,7 +22181,7 @@
         <v>8.0364989999999992</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -22295,7 +22289,7 @@
         <v>31.631349999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -22403,7 +22397,7 @@
         <v>23.576659999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -22511,7 +22505,7 @@
         <v>46.872069999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -22727,7 +22721,7 @@
         <v>22.130862</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -22835,7 +22829,7 @@
         <v>28.805669999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -22943,7 +22937,7 @@
         <v>35.490849999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -23051,7 +23045,7 @@
         <v>89.057860000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -23159,7 +23153,7 @@
         <v>36.906613000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -23267,7 +23261,7 @@
         <v>19.118648999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -23375,7 +23369,7 @@
         <v>53.959349999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -23483,7 +23477,7 @@
         <v>58.381350000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>2</v>
       </c>
@@ -23591,7 +23585,7 @@
         <v>149.67446999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>2</v>
       </c>
@@ -23807,7 +23801,7 @@
         <v>19.519779</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>3</v>
       </c>
@@ -23915,7 +23909,7 @@
         <v>34.34619</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>3</v>
       </c>
@@ -24023,7 +24017,7 @@
         <v>33.022220000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>3</v>
       </c>
@@ -24131,7 +24125,7 @@
         <v>33.776119999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>3</v>
       </c>
@@ -24239,7 +24233,7 @@
         <v>13.473632000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>3</v>
       </c>
@@ -24347,7 +24341,7 @@
         <v>32.749269999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>3</v>
       </c>
@@ -24455,7 +24449,7 @@
         <v>29.274169999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>3</v>
       </c>
@@ -24563,7 +24557,7 @@
         <v>26.385746000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>3</v>
       </c>
@@ -24671,7 +24665,7 @@
         <v>52.543216999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>3</v>
       </c>
@@ -24887,7 +24881,7 @@
         <v>34.390619999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>4</v>
       </c>
@@ -24995,7 +24989,7 @@
         <v>66.707520000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>4</v>
       </c>
@@ -25103,7 +25097,7 @@
         <v>70.819329999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>4</v>
       </c>
@@ -25211,7 +25205,7 @@
         <v>69.669430000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>4</v>
       </c>
@@ -25319,7 +25313,7 @@
         <v>189.44723000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>4</v>
       </c>
@@ -25427,7 +25421,7 @@
         <v>33.599119999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>4</v>
       </c>
@@ -25535,7 +25529,7 @@
         <v>52.688959999999994</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>4</v>
       </c>
@@ -25643,7 +25637,7 @@
         <v>44.101079999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>4</v>
       </c>
@@ -25751,7 +25745,7 @@
         <v>112.18261</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>4</v>
       </c>
@@ -25967,7 +25961,7 @@
         <v>40.06006</v>
       </c>
     </row>
-    <row r="42" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>5</v>
       </c>
@@ -26075,7 +26069,7 @@
         <v>56.237129999999993</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>5</v>
       </c>
@@ -26183,7 +26177,7 @@
         <v>32.144559999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>5</v>
       </c>
@@ -26291,7 +26285,7 @@
         <v>123.7513</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>5</v>
       </c>
@@ -26399,7 +26393,7 @@
         <v>31.325349999999993</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>5</v>
       </c>
@@ -26507,7 +26501,7 @@
         <v>11.419890000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>5</v>
       </c>
@@ -26615,7 +26609,7 @@
         <v>27.796389999999995</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>5</v>
       </c>
@@ -26723,7 +26717,7 @@
         <v>33.949210000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>5</v>
       </c>
@@ -26831,7 +26825,7 @@
         <v>76.908209999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>5</v>
       </c>
@@ -27047,7 +27041,7 @@
         <v>24.00244</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>6</v>
       </c>
@@ -27155,7 +27149,7 @@
         <v>21.794194000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>6</v>
       </c>
@@ -27263,7 +27257,7 @@
         <v>29.438233999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>6</v>
       </c>
@@ -27371,7 +27365,7 @@
         <v>63.986820000000009</v>
       </c>
     </row>
-    <row r="55" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>6</v>
       </c>
@@ -27479,7 +27473,7 @@
         <v>44.547850000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>6</v>
       </c>
@@ -27587,7 +27581,7 @@
         <v>17.9294443</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>6</v>
       </c>
@@ -27695,7 +27689,7 @@
         <v>78.487300000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>6</v>
       </c>
@@ -27803,7 +27797,7 @@
         <v>42.110354000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>6</v>
       </c>
@@ -27911,7 +27905,7 @@
         <v>187.26070000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>6</v>
       </c>
@@ -28127,7 +28121,7 @@
         <v>17.727543999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>7</v>
       </c>
@@ -28235,7 +28229,7 @@
         <v>64.894530000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>7</v>
       </c>
@@ -28343,7 +28337,7 @@
         <v>24.268557000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>7</v>
       </c>
@@ -28451,7 +28445,7 @@
         <v>53.006829999999994</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>7</v>
       </c>
@@ -28559,7 +28553,7 @@
         <v>10.731445000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>7</v>
       </c>
@@ -28667,7 +28661,7 @@
         <v>3.0644530000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>7</v>
       </c>
@@ -28775,7 +28769,7 @@
         <v>52.628900000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>7</v>
       </c>
@@ -28883,7 +28877,7 @@
         <v>40.296880000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>7</v>
       </c>
@@ -28991,7 +28985,7 @@
         <v>75.046880000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>7</v>
       </c>
@@ -29207,7 +29201,7 @@
         <v>22.77929</v>
       </c>
     </row>
-    <row r="72" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>8</v>
       </c>
@@ -29315,7 +29309,7 @@
         <v>238.83179000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>8</v>
       </c>
@@ -29423,7 +29417,7 @@
         <v>63.143549999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>8</v>
       </c>
@@ -29531,7 +29525,7 @@
         <v>34.204588000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>8</v>
       </c>
@@ -29639,7 +29633,7 @@
         <v>14.429200000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>8</v>
       </c>
@@ -29747,7 +29741,7 @@
         <v>7.6931149999999988</v>
       </c>
     </row>
-    <row r="77" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>8</v>
       </c>
@@ -29855,7 +29849,7 @@
         <v>28.822024000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>8</v>
       </c>
@@ -29963,7 +29957,7 @@
         <v>21.449705999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>8</v>
       </c>
@@ -30071,7 +30065,7 @@
         <v>51.211909999999996</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>8</v>
       </c>
@@ -30287,7 +30281,7 @@
         <v>17.880369000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>9</v>
       </c>
@@ -30395,7 +30389,7 @@
         <v>14.152832</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>9</v>
       </c>
@@ -30503,7 +30497,7 @@
         <v>14.733886</v>
       </c>
     </row>
-    <row r="84" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>9</v>
       </c>
@@ -30611,7 +30605,7 @@
         <v>34.413578000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>9</v>
       </c>
@@ -30719,7 +30713,7 @@
         <v>20.662593999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>9</v>
       </c>
@@ -30827,7 +30821,7 @@
         <v>29.100096000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>9</v>
       </c>
@@ -30935,7 +30929,7 @@
         <v>16.090328</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>9</v>
       </c>
@@ -31043,7 +31037,7 @@
         <v>35.551752999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>9</v>
       </c>
@@ -31151,7 +31145,7 @@
         <v>32.151367000000008</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>9</v>
       </c>
@@ -31367,7 +31361,7 @@
         <v>46.100089999999994</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>10</v>
       </c>
@@ -31475,7 +31469,7 @@
         <v>166.64652000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>10</v>
       </c>
@@ -31583,7 +31577,7 @@
         <v>51.654300000000006</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>10</v>
       </c>
@@ -31691,7 +31685,7 @@
         <v>248.64452</v>
       </c>
     </row>
-    <row r="95" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>10</v>
       </c>
@@ -31799,7 +31793,7 @@
         <v>24.703120999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>10</v>
       </c>
@@ -31907,7 +31901,7 @@
         <v>7.8652340000000009</v>
       </c>
     </row>
-    <row r="97" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>10</v>
       </c>
@@ -32015,7 +32009,7 @@
         <v>28.289065000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>10</v>
       </c>
@@ -32123,7 +32117,7 @@
         <v>28.154294</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>10</v>
       </c>
@@ -32231,7 +32225,7 @@
         <v>74.283204999999995</v>
       </c>
     </row>
-    <row r="100" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:33" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>10</v>
       </c>
@@ -32448,7 +32442,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE101" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <autoFilter ref="A1:AE101" xr:uid="{00000000-0001-0000-0400-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="7"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>